<commit_message>
Add Twitter API's analysis and project's hours + update planning and specifications.
</commit_message>
<xml_diff>
--- a/doc/planning/planification_gant_initiale.xlsx
+++ b/doc/planning/planification_gant_initiale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>GANTT</t>
   </si>
@@ -184,40 +184,46 @@
     <t>Schéma UML de l'application</t>
   </si>
   <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>Maquette UI</t>
+  </si>
+  <si>
     <t>Conception des fonctionnalités de base</t>
   </si>
   <si>
-    <t>T11</t>
+    <t>T12</t>
   </si>
   <si>
     <t>Module de récupération des Tweets</t>
   </si>
   <si>
-    <t>T12</t>
+    <t>T13</t>
   </si>
   <si>
     <t>Module d'analyse des Tweets récupérés</t>
   </si>
   <si>
-    <t>T13</t>
+    <t>T14</t>
   </si>
   <si>
     <t>Développement des bases de l'interface Web</t>
   </si>
   <si>
-    <t>T13-1</t>
+    <t>T14-1</t>
   </si>
   <si>
     <t>          Recherche de Tweets via mots-clés</t>
   </si>
   <si>
-    <t>T13-2</t>
+    <t>T14-2</t>
   </si>
   <si>
     <t>          Visualisation des résultats, sans carte</t>
   </si>
   <si>
-    <t>T13-3</t>
+    <t>T14-3</t>
   </si>
   <si>
     <t>          GUI</t>
@@ -226,40 +232,40 @@
     <t>Conception des fonctionnalités avancées</t>
   </si>
   <si>
-    <t>T14</t>
+    <t>T15</t>
   </si>
   <si>
     <t>Développement avancé de l'interface Web</t>
   </si>
   <si>
-    <t>T14-1</t>
+    <t>T15-1</t>
   </si>
   <si>
     <t>          Filtrage des recherches par région(s)</t>
   </si>
   <si>
-    <t>T14-2</t>
+    <t>T15-2</t>
   </si>
   <si>
     <t>          Visualisation des résultats sur la carte</t>
   </si>
   <si>
-    <t>T14-3</t>
+    <t>T15-3</t>
   </si>
   <si>
     <t>          Interaction avec la carte</t>
   </si>
   <si>
-    <t>T14-4</t>
-  </si>
-  <si>
-    <t>T15</t>
+    <t>T15-4</t>
+  </si>
+  <si>
+    <t>T16</t>
   </si>
   <si>
     <t>Développement de l'algorithme de clustering</t>
   </si>
   <si>
-    <t>T16</t>
+    <t>T17</t>
   </si>
   <si>
     <t>Divers (aide, page « about », etc.)</t>
@@ -268,19 +274,19 @@
     <t>Tests et validation</t>
   </si>
   <si>
-    <t>T17</t>
+    <t>T18</t>
   </si>
   <si>
     <t>Tests unitaires</t>
   </si>
   <si>
-    <t>T18</t>
+    <t>T19</t>
   </si>
   <si>
     <t>Tests fonctionnels</t>
   </si>
   <si>
-    <t>T19</t>
+    <t>T20</t>
   </si>
   <si>
     <t>Tests finaux</t>
@@ -651,7 +657,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -829,6 +835,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -992,11 +1002,11 @@
   <dimension ref="A1:AB65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1487,7 +1497,7 @@
       <c r="B13" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="20" t="s">
         <v>47</v>
       </c>
       <c r="D13" s="33" t="n">
@@ -1554,11 +1564,11 @@
       <c r="AA14" s="37"/>
       <c r="AB14" s="37"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="45" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="37" t="n">
@@ -1603,8 +1613,8 @@
       <c r="F16" s="23"/>
       <c r="G16" s="35"/>
       <c r="H16" s="24"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="0"/>
       <c r="K16" s="18"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23"/>
@@ -1625,28 +1635,30 @@
       <c r="AB16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="31"/>
+      <c r="B17" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22" t="n">
-        <v>5</v>
-      </c>
-      <c r="E17" s="42"/>
+      <c r="C17" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="35"/>
       <c r="H17" s="24"/>
       <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="J17" s="44"/>
       <c r="K17" s="18"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="24"/>
       <c r="S17" s="23"/>
       <c r="T17" s="23"/>
       <c r="U17" s="23"/>
@@ -1659,30 +1671,28 @@
       <c r="AB17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="46"/>
-      <c r="B18" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="48" t="s">
+      <c r="A18" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="49" t="n">
-        <v>1</v>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22" t="n">
+        <v>5</v>
       </c>
       <c r="E18" s="42"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="35"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="24"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
       <c r="K18" s="18"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="23"/>
       <c r="S18" s="23"/>
       <c r="T18" s="23"/>
       <c r="U18" s="23"/>
@@ -1695,30 +1705,30 @@
       <c r="AB18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47" t="s">
+      <c r="A19" s="47"/>
+      <c r="B19" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="49" t="n">
-        <v>2</v>
+      <c r="D19" s="50" t="n">
+        <v>1</v>
       </c>
       <c r="E19" s="42"/>
       <c r="F19" s="23"/>
       <c r="G19" s="35"/>
       <c r="H19" s="24"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
       <c r="K19" s="18"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="24"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
       <c r="S19" s="23"/>
       <c r="T19" s="23"/>
       <c r="U19" s="23"/>
@@ -1731,25 +1741,25 @@
       <c r="AB19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31"/>
-      <c r="B20" s="32" t="s">
+      <c r="A20" s="47"/>
+      <c r="B20" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="51" t="n">
-        <v>4</v>
-      </c>
-      <c r="E20" s="3"/>
+      <c r="D20" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="42"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="24"/>
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
       <c r="K20" s="18"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
       <c r="N20" s="23"/>
       <c r="O20" s="23"/>
       <c r="P20" s="23"/>
@@ -1771,25 +1781,25 @@
       <c r="B21" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="53" t="n">
-        <v>2</v>
+      <c r="D21" s="52" t="n">
+        <v>4</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="23"/>
-      <c r="G21" s="35"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="24"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
       <c r="K21" s="18"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
       <c r="P21" s="23"/>
-      <c r="Q21" s="37"/>
+      <c r="Q21" s="23"/>
       <c r="R21" s="24"/>
       <c r="S21" s="23"/>
       <c r="T21" s="23"/>
@@ -1807,11 +1817,11 @@
       <c r="B22" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="53" t="n">
-        <v>3</v>
+      <c r="D22" s="54" t="n">
+        <v>2</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="23"/>
@@ -1822,9 +1832,9 @@
       <c r="K22" s="18"/>
       <c r="L22" s="35"/>
       <c r="M22" s="35"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="51"/>
+      <c r="P22" s="23"/>
       <c r="Q22" s="37"/>
       <c r="R22" s="24"/>
       <c r="S22" s="23"/>
@@ -1838,122 +1848,122 @@
       <c r="AA22" s="23"/>
       <c r="AB22" s="23"/>
     </row>
-    <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="31"/>
       <c r="B23" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="53" t="n">
-        <v>4</v>
-      </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
+      <c r="D23" s="54" t="n">
+        <v>3</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="35"/>
       <c r="H23" s="24"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
       <c r="Q23" s="37"/>
       <c r="R23" s="24"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="25"/>
-      <c r="U23" s="25"/>
-      <c r="V23" s="25"/>
-      <c r="W23" s="25"/>
-      <c r="X23" s="25"/>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="25"/>
-      <c r="AA23" s="25"/>
-      <c r="AB23" s="25"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="21" t="s">
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+    </row>
+    <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="31"/>
+      <c r="B24" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22" t="n">
+      <c r="C24" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="54" t="n">
+        <v>4</v>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="25"/>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="25"/>
+      <c r="Z24" s="25"/>
+      <c r="AA24" s="25"/>
+      <c r="AB24" s="25"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="55"/>
-      <c r="S24" s="55"/>
-      <c r="T24" s="55"/>
-      <c r="U24" s="55"/>
-      <c r="V24" s="55"/>
-      <c r="W24" s="55"/>
-      <c r="X24" s="55"/>
-      <c r="Y24" s="37"/>
-      <c r="Z24" s="23"/>
-      <c r="AA24" s="23"/>
-      <c r="AB24" s="23"/>
-    </row>
-    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="56" t="n">
+      <c r="E25" s="3"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="56"/>
+      <c r="S25" s="56"/>
+      <c r="T25" s="56"/>
+      <c r="U25" s="56"/>
+      <c r="V25" s="56"/>
+      <c r="W25" s="56"/>
+      <c r="X25" s="56"/>
+      <c r="Y25" s="37"/>
+      <c r="Z25" s="23"/>
+      <c r="AA25" s="23"/>
+      <c r="AB25" s="23"/>
+    </row>
+    <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="47"/>
+      <c r="B26" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="57" t="n">
         <v>5</v>
-      </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="25"/>
-      <c r="S25" s="25"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="25"/>
-      <c r="V25" s="25"/>
-      <c r="W25" s="25"/>
-      <c r="X25" s="25"/>
-      <c r="Y25" s="37"/>
-      <c r="Z25" s="25"/>
-      <c r="AA25" s="25"/>
-      <c r="AB25" s="25"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="49" t="n">
-        <v>1</v>
       </c>
       <c r="E26" s="34"/>
       <c r="F26" s="25"/>
@@ -1967,7 +1977,7 @@
       <c r="N26" s="35"/>
       <c r="O26" s="35"/>
       <c r="P26" s="35"/>
-      <c r="Q26" s="57"/>
+      <c r="Q26" s="24"/>
       <c r="R26" s="25"/>
       <c r="S26" s="25"/>
       <c r="T26" s="25"/>
@@ -1981,15 +1991,15 @@
       <c r="AB26" s="25"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32" t="s">
+      <c r="A27" s="47"/>
+      <c r="B27" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="53" t="n">
-        <v>3</v>
+      <c r="D27" s="50" t="n">
+        <v>1</v>
       </c>
       <c r="E27" s="34"/>
       <c r="F27" s="25"/>
@@ -2000,13 +2010,13 @@
       <c r="K27" s="18"/>
       <c r="L27" s="25"/>
       <c r="M27" s="35"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
       <c r="P27" s="35"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
-      <c r="T27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
       <c r="U27" s="25"/>
       <c r="V27" s="25"/>
       <c r="W27" s="25"/>
@@ -2021,10 +2031,10 @@
       <c r="B28" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C28" s="52" t="s">
+      <c r="C28" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="53" t="n">
+      <c r="D28" s="54" t="n">
         <v>3</v>
       </c>
       <c r="E28" s="34"/>
@@ -2035,15 +2045,15 @@
       <c r="J28" s="25"/>
       <c r="K28" s="18"/>
       <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
+      <c r="M28" s="35"/>
       <c r="N28" s="25"/>
       <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
+      <c r="P28" s="35"/>
       <c r="Q28" s="24"/>
-      <c r="R28" s="25"/>
-      <c r="S28" s="58"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="58"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="59"/>
+      <c r="T28" s="59"/>
+      <c r="U28" s="25"/>
       <c r="V28" s="25"/>
       <c r="W28" s="25"/>
       <c r="X28" s="25"/>
@@ -2057,11 +2067,11 @@
       <c r="B29" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="53" t="n">
-        <v>5</v>
+      <c r="C29" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="54" t="n">
+        <v>3</v>
       </c>
       <c r="E29" s="34"/>
       <c r="F29" s="25"/>
@@ -2075,11 +2085,11 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
       <c r="P29" s="25"/>
-      <c r="Q29" s="57"/>
-      <c r="R29" s="58"/>
-      <c r="S29" s="58"/>
-      <c r="T29" s="58"/>
-      <c r="U29" s="58"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="59"/>
+      <c r="U29" s="59"/>
       <c r="V29" s="25"/>
       <c r="W29" s="25"/>
       <c r="X29" s="25"/>
@@ -2091,13 +2101,13 @@
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="31"/>
       <c r="B30" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="53" t="n">
-        <v>3</v>
+      <c r="C30" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="54" t="n">
+        <v>5</v>
       </c>
       <c r="E30" s="34"/>
       <c r="F30" s="25"/>
@@ -2111,16 +2121,16 @@
       <c r="N30" s="25"/>
       <c r="O30" s="25"/>
       <c r="P30" s="25"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="58"/>
-      <c r="V30" s="58"/>
-      <c r="W30" s="58"/>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="59"/>
+      <c r="S30" s="59"/>
+      <c r="T30" s="59"/>
+      <c r="U30" s="59"/>
+      <c r="V30" s="25"/>
+      <c r="W30" s="25"/>
       <c r="X30" s="25"/>
       <c r="Y30" s="37"/>
-      <c r="Z30" s="37"/>
+      <c r="Z30" s="25"/>
       <c r="AA30" s="25"/>
       <c r="AB30" s="25"/>
     </row>
@@ -2129,11 +2139,11 @@
       <c r="B31" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="53" t="n">
-        <v>1</v>
+      <c r="D31" s="54" t="n">
+        <v>3</v>
       </c>
       <c r="E31" s="34"/>
       <c r="F31" s="25"/>
@@ -2151,86 +2161,86 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
       <c r="T31" s="25"/>
-      <c r="U31" s="25"/>
-      <c r="V31" s="25"/>
-      <c r="W31" s="25"/>
-      <c r="X31" s="58"/>
+      <c r="U31" s="59"/>
+      <c r="V31" s="59"/>
+      <c r="W31" s="59"/>
+      <c r="X31" s="25"/>
       <c r="Y31" s="37"/>
       <c r="Z31" s="37"/>
       <c r="AA31" s="25"/>
       <c r="AB31" s="25"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="31"/>
+      <c r="B32" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22" t="n">
+      <c r="C32" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="34"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="25"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="25"/>
+      <c r="V32" s="25"/>
+      <c r="W32" s="25"/>
+      <c r="X32" s="59"/>
+      <c r="Y32" s="37"/>
+      <c r="Z32" s="37"/>
+      <c r="AA32" s="25"/>
+      <c r="AB32" s="25"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="59"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="60"/>
-      <c r="P32" s="60"/>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="61"/>
-      <c r="S32" s="59"/>
-      <c r="T32" s="59"/>
-      <c r="U32" s="59"/>
-      <c r="V32" s="59"/>
-      <c r="W32" s="59"/>
-      <c r="X32" s="59"/>
-      <c r="Y32" s="59"/>
-      <c r="Z32" s="59"/>
-      <c r="AA32" s="23"/>
-      <c r="AB32" s="23"/>
-    </row>
-    <row r="33" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="33" t="n">
-        <v>13</v>
-      </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
       <c r="H33" s="24"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="62"/>
-      <c r="N33" s="62"/>
-      <c r="O33" s="62"/>
-      <c r="P33" s="62"/>
-      <c r="Q33" s="62"/>
-      <c r="R33" s="63"/>
-      <c r="S33" s="62"/>
-      <c r="T33" s="62"/>
-      <c r="U33" s="62"/>
-      <c r="V33" s="62"/>
-      <c r="W33" s="62"/>
-      <c r="X33" s="62"/>
-      <c r="Y33" s="25"/>
-      <c r="Z33" s="25"/>
-      <c r="AA33" s="25"/>
-      <c r="AB33" s="25"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L33" s="60"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="61"/>
+      <c r="P33" s="61"/>
+      <c r="Q33" s="61"/>
+      <c r="R33" s="62"/>
+      <c r="S33" s="60"/>
+      <c r="T33" s="60"/>
+      <c r="U33" s="60"/>
+      <c r="V33" s="60"/>
+      <c r="W33" s="60"/>
+      <c r="X33" s="60"/>
+      <c r="Y33" s="60"/>
+      <c r="Z33" s="60"/>
+      <c r="AA33" s="23"/>
+      <c r="AB33" s="23"/>
+    </row>
+    <row r="34" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="31"/>
       <c r="B34" s="32" t="s">
         <v>84</v>
@@ -2239,7 +2249,7 @@
         <v>85</v>
       </c>
       <c r="D34" s="33" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E34" s="34"/>
       <c r="F34" s="25"/>
@@ -2248,19 +2258,19 @@
       <c r="I34" s="25"/>
       <c r="J34" s="25"/>
       <c r="K34" s="18"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="62"/>
-      <c r="O34" s="62"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="62"/>
-      <c r="R34" s="63"/>
-      <c r="S34" s="62"/>
-      <c r="T34" s="62"/>
-      <c r="U34" s="62"/>
-      <c r="V34" s="62"/>
-      <c r="W34" s="62"/>
-      <c r="X34" s="62"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="63"/>
+      <c r="O34" s="63"/>
+      <c r="P34" s="63"/>
+      <c r="Q34" s="63"/>
+      <c r="R34" s="64"/>
+      <c r="S34" s="63"/>
+      <c r="T34" s="63"/>
+      <c r="U34" s="63"/>
+      <c r="V34" s="63"/>
+      <c r="W34" s="63"/>
+      <c r="X34" s="63"/>
       <c r="Y34" s="25"/>
       <c r="Z34" s="25"/>
       <c r="AA34" s="25"/>
@@ -2275,7 +2285,7 @@
         <v>87</v>
       </c>
       <c r="D35" s="33" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E35" s="34"/>
       <c r="F35" s="25"/>
@@ -2286,56 +2296,91 @@
       <c r="K35" s="18"/>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="25"/>
-      <c r="T35" s="25"/>
-      <c r="U35" s="25"/>
-      <c r="V35" s="25"/>
-      <c r="W35" s="25"/>
-      <c r="X35" s="25"/>
-      <c r="Y35" s="62"/>
-      <c r="Z35" s="62"/>
+      <c r="N35" s="63"/>
+      <c r="O35" s="63"/>
+      <c r="P35" s="63"/>
+      <c r="Q35" s="63"/>
+      <c r="R35" s="64"/>
+      <c r="S35" s="63"/>
+      <c r="T35" s="63"/>
+      <c r="U35" s="63"/>
+      <c r="V35" s="63"/>
+      <c r="W35" s="63"/>
+      <c r="X35" s="63"/>
+      <c r="Y35" s="25"/>
+      <c r="Z35" s="25"/>
       <c r="AA35" s="25"/>
       <c r="AB35" s="25"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="31"/>
+      <c r="B36" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="22" t="n">
+      <c r="C36" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="37"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="37"/>
-      <c r="O36" s="37"/>
-      <c r="P36" s="37"/>
-      <c r="Q36" s="37"/>
-      <c r="R36" s="37"/>
-      <c r="S36" s="37"/>
-      <c r="T36" s="37"/>
-      <c r="U36" s="37"/>
-      <c r="V36" s="37"/>
-      <c r="W36" s="37"/>
-      <c r="X36" s="37"/>
-      <c r="Y36" s="37"/>
-      <c r="Z36" s="37"/>
-      <c r="AA36" s="64"/>
-      <c r="AB36" s="64"/>
-    </row>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="25"/>
+      <c r="T36" s="25"/>
+      <c r="U36" s="25"/>
+      <c r="V36" s="25"/>
+      <c r="W36" s="25"/>
+      <c r="X36" s="25"/>
+      <c r="Y36" s="63"/>
+      <c r="Z36" s="63"/>
+      <c r="AA36" s="25"/>
+      <c r="AB36" s="25"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
+      <c r="W37" s="37"/>
+      <c r="X37" s="37"/>
+      <c r="Y37" s="37"/>
+      <c r="Z37" s="37"/>
+      <c r="AA37" s="65"/>
+      <c r="AB37" s="65"/>
+    </row>
     <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2387,14 +2432,14 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="F2:AB2"/>
-    <mergeCell ref="K3:K36"/>
+    <mergeCell ref="K3:K37"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>